<commit_message>
Campio de dias de garcia en unidades nuevas
Campio de dias de garcia en unidades nuevas
</commit_message>
<xml_diff>
--- a/files/LayoutUnidades.xlsx
+++ b/files/LayoutUnidades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Mis documentos\GitHub\planPiso\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F84A7F9-4581-40B7-A2DB-0BB9A2385F14}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E4F5319-C83E-4CBE-A3CD-CB1BF245F2DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="9165" windowWidth="29040" windowHeight="15840" xr2:uid="{1ADB4FD7-A697-46A7-86D6-8EA9EEB47067}"/>
+    <workbookView xWindow="-28920" yWindow="7395" windowWidth="29040" windowHeight="15840" xr2:uid="{1ADB4FD7-A697-46A7-86D6-8EA9EEB47067}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Numeroserie</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>Fecha</t>
+  </si>
+  <si>
+    <t>Gracia</t>
   </si>
 </sst>
 </file>
@@ -89,10 +92,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -131,12 +135,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B8421711-38AC-4A70-BAEF-373FDDC4E814}" name="Tabla1" displayName="Tabla1" ref="A1:C4" totalsRowShown="0">
-  <autoFilter ref="A1:C4" xr:uid="{C664C210-EE0F-46A0-9C7E-E6090001C800}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B8421711-38AC-4A70-BAEF-373FDDC4E814}" name="Tabla1" displayName="Tabla1" ref="A1:D4" totalsRowShown="0">
+  <autoFilter ref="A1:D4" xr:uid="{C664C210-EE0F-46A0-9C7E-E6090001C800}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{97CD01A3-7B84-4021-B2AB-A2BBAF1D572B}" name="Numeroserie"/>
     <tableColumn id="2" xr3:uid="{C99A62E6-FEF0-4734-A75D-397472FC07D5}" name="Valor" dataDxfId="0" dataCellStyle="Millares"/>
     <tableColumn id="3" xr3:uid="{3C8487B3-1545-4A58-9812-91DB5DD16850}" name="Fecha"/>
+    <tableColumn id="4" xr3:uid="{8FEEE104-9D6D-40D8-B5AD-7357F0BC6F97}" name="Gracia"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -439,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B48DF34-8E4D-4AFF-846F-BD0853CBA404}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,7 +455,7 @@
     <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -460,8 +465,11 @@
       <c r="C1" t="s">
         <v>5</v>
       </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -471,8 +479,11 @@
       <c r="C2" s="2">
         <v>44256</v>
       </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -482,8 +493,11 @@
       <c r="C3" s="2">
         <v>44260</v>
       </c>
+      <c r="D3" s="3">
+        <v>30</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -492,6 +506,9 @@
       </c>
       <c r="C4" s="2">
         <v>44260</v>
+      </c>
+      <c r="D4">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>